<commit_message>
fix: correct framecount to duration calculation for 29.97 and 59.94 framerates
</commit_message>
<xml_diff>
--- a/timecode.xlsx
+++ b/timecode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Documents/Work/hootworks/clients/all3media/timecodes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/projects/vectronic/timecode-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2902C981-7923-554A-9924-2A31D30C43D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E90F5C-05D8-4146-8BAE-AF00211423C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="36760" windowHeight="18480" xr2:uid="{89A11EBA-0812-1947-BD4D-CE0C8900BDA1}"/>
   </bookViews>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -822,7 +825,7 @@
   <dimension ref="B1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,14 +955,14 @@
         <v>23</v>
       </c>
       <c r="D3" s="18">
-        <f>1000000/(C3+1)</f>
-        <v>41666.666666666664</v>
+        <f>1000000/23.976</f>
+        <v>41708.375041708379</v>
       </c>
       <c r="E3" s="19">
         <v>0</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="29"/>
       <c r="I3" s="32" t="s">
@@ -978,7 +981,7 @@
       </c>
       <c r="M3" s="48">
         <f>L3 * LOOKUP($G$3, $B$3:$B$13, $D$3:$D$13)</f>
-        <v>10000000</v>
+        <v>10010010.010010011</v>
       </c>
       <c r="N3" s="30">
         <v>1020304</v>
@@ -993,7 +996,7 @@
       </c>
       <c r="Q3" s="48">
         <f>P3 * LOOKUP($G$3, $B$3:$B$13, $D$3:$D$13)</f>
-        <v>3723133333.3333335</v>
+        <v>3726860193.5268602</v>
       </c>
       <c r="R3" s="26">
         <f>O3-K3</f>
@@ -1005,7 +1008,7 @@
       </c>
       <c r="T3" s="43">
         <f>S3 * LOOKUP($G$3, $B$3:$B$13, $D$3:$D$13)</f>
-        <v>3713133333.3333335</v>
+        <v>3716850183.5168505</v>
       </c>
       <c r="U3" s="6">
         <f>INT(TEXT(TRUNC(R3 / (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), "00") &amp; TEXT(TRUNC(MOD(R3, (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))) / (60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), "00") &amp; TEXT(TRUNC(MOD(MOD(R3, (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), (60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))) / (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1)), "00") &amp; TEXT(MOD(MOD(MOD(R3, (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), (60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1)), "00"))</f>
@@ -1044,7 +1047,7 @@
       </c>
       <c r="M4" s="48">
         <f t="shared" ref="M4:M13" si="4">L4 * LOOKUP($G$3, $B$3:$B$13, $D$3:$D$13)</f>
-        <v>35990633333.333336</v>
+        <v>36026659993.32666</v>
       </c>
       <c r="N4" s="30">
         <v>9595710</v>
@@ -1059,7 +1062,7 @@
       </c>
       <c r="Q4" s="48">
         <f t="shared" ref="Q4:Q13" si="6">P4 * LOOKUP($G$3, $B$3:$B$13, $D$3:$D$13)</f>
-        <v>35997333333.333336</v>
+        <v>36033366700.033371</v>
       </c>
       <c r="R4" s="26">
         <f t="shared" ref="R4:R13" si="7">O4-K4</f>
@@ -1071,7 +1074,7 @@
       </c>
       <c r="T4" s="43">
         <f t="shared" ref="T4:T13" si="9">Q4-M4</f>
-        <v>6700000</v>
+        <v>6706706.7067108154</v>
       </c>
       <c r="U4" s="6">
         <f t="shared" ref="U4:U13" si="10">INT(TEXT(TRUNC(R4 / (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), "00") &amp; TEXT(TRUNC(MOD(R4, (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))) / (60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), "00") &amp; TEXT(TRUNC(MOD(MOD(R4, (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), (60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))) / (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1)), "00") &amp; TEXT(MOD(MOD(MOD(R4, (60 * 60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), (60 * (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1))), (LOOKUP($G$3, $B$3:$B$13, $C$3:$C$13) + 1)), "00"))</f>
@@ -1110,7 +1113,7 @@
       </c>
       <c r="M5" s="48">
         <f t="shared" si="4"/>
-        <v>35997333333.333336</v>
+        <v>36033366700.033371</v>
       </c>
       <c r="N5" s="30">
         <v>10000000</v>
@@ -1125,7 +1128,7 @@
       </c>
       <c r="Q5" s="48">
         <f t="shared" si="6"/>
-        <v>36000000000</v>
+        <v>36036036036.036041</v>
       </c>
       <c r="R5" s="26">
         <f t="shared" si="7"/>
@@ -1137,7 +1140,7 @@
       </c>
       <c r="T5" s="43">
         <f t="shared" si="9"/>
-        <v>2666666.6666641235</v>
+        <v>2669336.0026702881</v>
       </c>
       <c r="U5" s="6">
         <f t="shared" si="10"/>
@@ -1152,8 +1155,8 @@
         <v>29</v>
       </c>
       <c r="D6" s="18">
-        <f>1000000/(30000/1001)</f>
-        <v>33366.666666666664</v>
+        <f>1000000/29.97</f>
+        <v>33366.700033366702</v>
       </c>
       <c r="E6" s="19">
         <v>2</v>
@@ -1176,7 +1179,7 @@
       </c>
       <c r="M6" s="48">
         <f t="shared" si="4"/>
-        <v>36000333333.333336</v>
+        <v>36036369703.036369</v>
       </c>
       <c r="N6" s="30">
         <v>10254010</v>
@@ -1191,7 +1194,7 @@
       </c>
       <c r="Q6" s="48">
         <f t="shared" si="6"/>
-        <v>37540333333.333336</v>
+        <v>37577911244.577911</v>
       </c>
       <c r="R6" s="27">
         <f t="shared" si="7"/>
@@ -1203,7 +1206,7 @@
       </c>
       <c r="T6" s="43">
         <f t="shared" si="9"/>
-        <v>1540000000</v>
+        <v>1541541541.5415421</v>
       </c>
       <c r="U6" s="6">
         <f t="shared" si="10"/>
@@ -1218,8 +1221,8 @@
         <v>29</v>
       </c>
       <c r="D7" s="18">
-        <f>1000000/(30000/1001)</f>
-        <v>33366.666666666664</v>
+        <f>1000000/29.97</f>
+        <v>33366.700033366702</v>
       </c>
       <c r="E7" s="19">
         <v>0</v>
@@ -1230,19 +1233,19 @@
         <v>25</v>
       </c>
       <c r="J7" s="30">
-        <v>10254010</v>
+        <v>22000000</v>
       </c>
       <c r="K7" s="27">
         <f t="shared" si="2"/>
-        <v>1126210</v>
+        <v>2376000</v>
       </c>
       <c r="L7" s="47">
         <f t="shared" si="3"/>
-        <v>1126210</v>
+        <v>2376000</v>
       </c>
       <c r="M7" s="48">
         <f t="shared" si="4"/>
-        <v>37540333333.333336</v>
+        <v>79279279279.279282</v>
       </c>
       <c r="N7" s="30">
         <v>10255010</v>
@@ -1257,23 +1260,23 @@
       </c>
       <c r="Q7" s="48">
         <f t="shared" si="6"/>
-        <v>37550333333.333336</v>
+        <v>37587921254.587921</v>
       </c>
       <c r="R7" s="27">
         <f t="shared" si="7"/>
-        <v>300</v>
+        <v>-1249490</v>
       </c>
       <c r="S7" s="27">
         <f t="shared" si="8"/>
-        <v>300</v>
+        <v>-1249490</v>
       </c>
       <c r="T7" s="43">
         <f t="shared" si="9"/>
-        <v>10000000</v>
+        <v>-41691358024.69136</v>
       </c>
       <c r="U7" s="6">
         <f t="shared" si="10"/>
-        <v>1000</v>
+        <v>-11255010</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
@@ -1476,8 +1479,8 @@
         <v>59</v>
       </c>
       <c r="D11" s="18">
-        <f>1000000/(60000/1001)</f>
-        <v>16683.333333333332</v>
+        <f>1000000/59.94</f>
+        <v>16683.350016683351</v>
       </c>
       <c r="E11" s="19">
         <v>4</v>
@@ -1540,8 +1543,8 @@
         <v>59</v>
       </c>
       <c r="D12" s="18">
-        <f>1000000/(60000/1001)</f>
-        <v>16683.333333333332</v>
+        <f>1000000/59.94</f>
+        <v>16683.350016683351</v>
       </c>
       <c r="E12" s="19">
         <v>0</v>

</xml_diff>